<commit_message>
Add support for derivative parameters to refer to themselves
</commit_message>
<xml_diff>
--- a/tests/framework_derivative_test.xlsx
+++ b/tests/framework_derivative_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27ABE9D7-65C9-447A-B68D-D3494C3299D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F98654-E256-4562-922E-D4BC04BDEA71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -569,7 +569,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>Datasheet Code Name</t>
   </si>
@@ -653,6 +653,15 @@
   </si>
   <si>
     <t>Mosquito prevalance</t>
+  </si>
+  <si>
+    <t>converge</t>
+  </si>
+  <si>
+    <t>Convergence test</t>
+  </si>
+  <si>
+    <t>1-converge</t>
   </si>
 </sst>
 </file>
@@ -5351,10 +5360,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5435,6 +5444,26 @@
         <v>25</v>
       </c>
       <c r="H3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>